<commit_message>
finalize cols per convo w steph
</commit_message>
<xml_diff>
--- a/export/GHS Tracking Dashboard - Project Report Template v2.xlsx
+++ b/export/GHS Tracking Dashboard - Project Report Template v2.xlsx
@@ -12,7 +12,7 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11685" xr2:uid="{E1F37E5D-701C-4E0F-9790-B519BA336093}"/>
   </bookViews>
   <sheets>
-    <sheet name="Template" sheetId="4" r:id="rId1"/>
+    <sheet name="Project report template" sheetId="4" r:id="rId1"/>
     <sheet name="Legend" sheetId="6" r:id="rId2"/>
     <sheet name="Do not edit - Column values" sheetId="5" r:id="rId3"/>
   </sheets>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="82">
   <si>
     <t>Transaction Amount</t>
   </si>
@@ -356,22 +356,6 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Transaction Type
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color rgb="FFFFFFFF"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(choose one or enter custom)</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t xml:space="preserve">Transaction Currency
 </t>
     </r>
@@ -403,54 +387,7 @@
     </r>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Recipient sector
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color rgb="FFFFFFFF"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(choose one or enter custom)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Funder sector
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color rgb="FFFFFFFF"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(choose one or enter custom)</t>
-    </r>
-  </si>
-  <si>
     <t>2017-2022</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Recipient information </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="22"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(enter once per project)</t>
-    </r>
   </si>
   <si>
     <r>
@@ -520,6 +457,41 @@
   </si>
   <si>
     <t>General IHR Implementation</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Government funder?
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFFFFFFF"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(choose one)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Government recipient?
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFFFFFFF"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(choose one)</t>
+    </r>
+  </si>
+  <si>
+    <t>Transactions</t>
   </si>
 </sst>
 </file>
@@ -782,7 +754,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -827,16 +799,15 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -846,14 +817,14 @@
     <xf numFmtId="0" fontId="5" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1255,7 +1226,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B5" sqref="B5"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1328,67 +1299,67 @@
       <c r="P3" s="10"/>
     </row>
     <row r="4" spans="1:16" ht="29.25" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A4" s="25" t="s">
+      <c r="A4" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="B4" s="26"/>
-      <c r="C4" s="26"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="22" t="s">
+      <c r="B4" s="19"/>
+      <c r="C4" s="19"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="G4" s="23"/>
-      <c r="H4" s="24"/>
-      <c r="I4" s="22" t="s">
-        <v>72</v>
+      <c r="G4" s="22"/>
+      <c r="H4" s="23"/>
+      <c r="I4" s="21" t="s">
+        <v>41</v>
       </c>
-      <c r="J4" s="23"/>
-      <c r="K4" s="24"/>
+      <c r="J4" s="22"/>
+      <c r="K4" s="23"/>
       <c r="L4" s="21" t="s">
-        <v>55</v>
+        <v>81</v>
       </c>
-      <c r="M4" s="21"/>
-      <c r="N4" s="21"/>
-      <c r="O4" s="21"/>
-      <c r="P4" s="21"/>
+      <c r="M4" s="22"/>
+      <c r="N4" s="22"/>
+      <c r="O4" s="22"/>
+      <c r="P4" s="23"/>
     </row>
     <row r="5" spans="1:16" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="16" t="s">
         <v>36</v>
       </c>
       <c r="B5" s="16" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C5" s="16" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="D5" s="16" t="s">
         <v>53</v>
       </c>
       <c r="E5" s="16" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="F5" s="17" t="s">
         <v>38</v>
       </c>
       <c r="G5" s="17" t="s">
-        <v>70</v>
+        <v>79</v>
       </c>
       <c r="H5" s="17" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="I5" s="16" t="s">
         <v>42</v>
       </c>
       <c r="J5" s="16" t="s">
-        <v>69</v>
+        <v>80</v>
       </c>
       <c r="K5" s="16" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="L5" s="17" t="s">
-        <v>66</v>
+        <v>46</v>
       </c>
       <c r="M5" s="17" t="s">
         <v>63</v>
@@ -1397,10 +1368,10 @@
         <v>0</v>
       </c>
       <c r="O5" s="17" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="P5" s="17" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="6" spans="1:16" ht="75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1408,7 +1379,7 @@
         <v>58</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>8</v>
@@ -1418,7 +1389,7 @@
         <v>32</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>60</v>
@@ -1427,7 +1398,7 @@
         <v>64</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="J6" s="1" t="s">
         <v>60</v>
@@ -1448,7 +1419,7 @@
         <v>6</v>
       </c>
       <c r="P6" s="3" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="7" spans="1:16" ht="75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1466,7 +1437,7 @@
         <v>32</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>60</v>
@@ -1475,7 +1446,7 @@
         <v>64</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="J7" s="1" t="s">
         <v>60</v>
@@ -28408,10 +28379,11 @@
       <c r="P1502" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="A4:E4"/>
     <mergeCell ref="F4:H4"/>
     <mergeCell ref="I4:K4"/>
+    <mergeCell ref="L4:P4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -28533,32 +28505,32 @@
       <c r="R3" s="10"/>
     </row>
     <row r="4" spans="1:18" ht="29.25" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A4" s="18" t="s">
+      <c r="A4" s="24" t="s">
         <v>45</v>
       </c>
-      <c r="B4" s="18"/>
-      <c r="C4" s="18"/>
-      <c r="D4" s="18"/>
-      <c r="E4" s="18"/>
-      <c r="F4" s="18"/>
-      <c r="G4" s="19"/>
-      <c r="H4" s="20" t="s">
+      <c r="B4" s="24"/>
+      <c r="C4" s="24"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="25"/>
+      <c r="H4" s="26" t="s">
         <v>37</v>
       </c>
-      <c r="I4" s="20"/>
-      <c r="J4" s="20"/>
-      <c r="K4" s="20" t="s">
+      <c r="I4" s="26"/>
+      <c r="J4" s="26"/>
+      <c r="K4" s="26" t="s">
         <v>41</v>
       </c>
-      <c r="L4" s="20"/>
-      <c r="M4" s="20"/>
-      <c r="N4" s="20" t="s">
+      <c r="L4" s="26"/>
+      <c r="M4" s="26"/>
+      <c r="N4" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="O4" s="20"/>
-      <c r="P4" s="20"/>
-      <c r="Q4" s="20"/>
-      <c r="R4" s="20"/>
+      <c r="O4" s="26"/>
+      <c r="P4" s="26"/>
+      <c r="Q4" s="26"/>
+      <c r="R4" s="26"/>
     </row>
     <row r="5" spans="1:18" ht="38.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="11" t="s">
@@ -58650,7 +58622,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8902F336-D6B1-4B22-A163-BA33346C1940}">
   <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -58696,7 +58670,7 @@
         <v>29</v>
       </c>
       <c r="C3" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="D3" t="s">
         <v>3</v>
@@ -58801,7 +58775,7 @@
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>

</xml_diff>